<commit_message>
Truly Final commit and check. Added "ready to be sent" version of the Self Assessment Form
</commit_message>
<xml_diff>
--- a/Self Assessment Form - IUM-TWEB.xlsx
+++ b/Self Assessment Form - IUM-TWEB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmar9\Desktop\TWEB_MARINO_814025_IUMTWEB12CFU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmar9\Desktop\TWEB_MARINO_814025_IUMTWEB12CFU\IUMTWEB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79D7560-52C9-4176-A8CB-D2F7E13BED16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D95F84-3D6C-4F3F-BD34-55B0A96BC376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{9384817B-0988-A24F-9D66-74DAD74AC274}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
   <si>
     <t>Team Name</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>Si, per ogni funzione, componente, richiesta, route ecc.. Ho inserito commenti e documentazione javadoc</t>
-  </si>
-  <si>
-    <t>Si, ho utilizzato inizialmente yaml ma poi sono passato all'utilizzo di json per i file della documentazione poiché molto più rapidi e di maggior qualità</t>
   </si>
   <si>
     <t>No.</t>
@@ -625,15 +622,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -641,6 +629,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="27" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -961,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A704EA58-8849-E44F-8AE0-CB0AA8314588}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -975,21 +972,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="36" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
       <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:5" s="36" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="51" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
       <c r="E2" s="43"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -1021,7 +1018,7 @@
       <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="48" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="2"/>
@@ -1481,9 +1478,6 @@
       <c r="D66">
         <v>3</v>
       </c>
-      <c r="E66" s="41" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B67" s="29" t="s">
@@ -1517,7 +1511,7 @@
       </c>
       <c r="C71" s="39"/>
       <c r="E71" s="41" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.4">
@@ -1555,7 +1549,7 @@
       <c r="D75" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E75" s="50"/>
+      <c r="E75" s="47"/>
     </row>
     <row r="76" spans="1:5" ht="73" x14ac:dyDescent="0.4">
       <c r="A76" s="34" t="s">
@@ -1563,7 +1557,7 @@
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
-      <c r="D76" s="49"/>
+      <c r="D76" s="46"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77" s="19"/>

</xml_diff>

<commit_message>
Added last version of IUM-TWEB, updated by removing the part where I was talking about the error on the games page ( solved some commits earlier today ).
</commit_message>
<xml_diff>
--- a/Self Assessment Form - IUM-TWEB.xlsx
+++ b/Self Assessment Form - IUM-TWEB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmar9\Desktop\TWEB_MARINO_814025_IUMTWEB12CFU\IUMTWEB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmar9\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D95F84-3D6C-4F3F-BD34-55B0A96BC376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A099A9A-6438-4BDC-B16D-592B998FDEAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{9384817B-0988-A24F-9D66-74DAD74AC274}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>Team Name</t>
   </si>
@@ -237,18 +237,9 @@
     <t>Mi sono avvalso di un’ampia gamma di fonti tra cui W3Schools, forum per sviluppatori come Stack Overflow, la documentazione di Socket.io, ReactJS e MUI-Library per i componenti MUI</t>
   </si>
   <si>
-    <t>Alcune partite presenti nel dataset vengono trasmesse con alcune mancanze, ovvero i giocatori non sono presenti nella timeline delle azioni ma lo sono invece in quella delle formazioni o viceversa ( probabilmente dovuta a delle mancanze proprie dei dataset ), inoltre pur essendo presenti partite fino al 2012, sul calendario in games vengono mostrate solo dal 2022 al 2023 con alcune partite nel 2021 e nel 2019. Questo però non si presenta se si va a cercare le partite giocate dal club o dal giocatore, ove invece sono visibili tutte le partite anche di anni precedenti o successivi a quelli indicati sopra ( escluso il 2024 poichè il dataset non ne contiene )</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vedi mongo DB </t>
-  </si>
-  <si>
     <t>Ho sviluppato la webapp utilizzando React , una libreria open-source, front-end e JavaScript per la creazione di interfacce utente di proprietà di META, suddividendola in pagine che però rispettano le richieste di sviluppo fornite dall'Assignment Document ( ovvero creare un one-page website ), assieme a MUI-Library e a diversi fogli di stile per quanto riguarda invece il look del sito . Successivamente ho deciso di suddividere le pagine in più livelli, implementando quindi una struttura modulare e organizzando il codice seguendo una gerarchia di componenti, composti in alcuni casi anche da atomi e card. Ho inoltre implementato il sistema di autenticazione suddividendolo in due macro componenti, Login e Signup, e numerosi microcomponenti e atomi. Per quanto riguarda Signup esso è  collegato a UserService, servizio per gestire la chiamata axios fatta durante la registrazione dell'utente nel sito, ed ai componenti alerterror e alertsuccess che mostrano su schermo notifiche di errore o di successo nell'autenticazione. Login invece presenta un componente di nome AuthContext che, tramite la chiamata user-credentials, riceve dal database le credenziali aggiunte con signup collegate all'utente e permette l'accesso al sito. La chat è stata sviluppata usando WebSocket e Socket.io, è visibile solo dopo aver fatto login o essersi registrati tramite signup e presenta tre macrochatroom di nome "teamsroom", "playersroom" e "gamesroom" in cui poter comunicare con gli altri utenti del sito. Nella homepage del sito sono presenti link alle tre aree "Games", "Teams" e "Competitions" oltre che due sezioni contenenti le news in evidenza e altre news. Le due sezioni news fanno riferimento al servizio HomeService nel quale è presente una richiesta ad una API esterna, di proprietà di Google News, che si occupa di news calcistiche, e di cui viene fornita la chiave, a quale ha un limite giornaliero di 30-40 utilizzi poichè in versione free. Per quanto riguarda invece le altre tre pagine, ognuna di esse fa riferimento ai servizi ad esse dedicate, in particolare per "Teams" e "Competitions" ho sviluppato due pagine, di nome "Single-Team" e "Single-Competition" ( con servizi annessi ) che, come dice il nome, riguardano il singolo team o la singola competizione scelta nelle pagine precedenti. Le pagine sono comunicanti fra loro e in particolare quella dei Single-Team presenta oltre al box informativo anche due sottosezioni di nome "players" e "games" che mostrano i giocatori appartenenti alla squadra e le partite della stessa. Focalizzandoci su "players" è stata creata una pagina "single-player" che mostra tutte le informazioni del giocatore e le partite disputate ordinate per data. Cliccando su una qualsiasi partita si apre la pagina "single-game", raggiungibile anche dalla sezione delle partite giocate dal team selezionato, che mostra tutte le informazioni della singola partita tra cui azioni di gioco e formazioni divise in due sezioni. Ogni singolo nome di ogni singolo giocatore presente in ogni sezione porta, tramite click, alla pagina del giocatore. Le partite sono anche raggiungibili tramite la pagina "Games" la quale presenta un calendario navigabile sul quale, in presenza di partite nel giorno scelto ( indicato da un pallino sotto al numero del giorno ), è possibile cliccare per vedere tutte le partite giocatesi in quel giorno.</t>
   </si>
   <si>
-    <t>Per quanto riguarda MongoDB, ho utilizzato tale database per memorizzare dati dinamici e in rapida evoluzione, quali i dettagli delle partite, gli eventi di gioco, le partite dei club e le prestazioni dei giocatori nelle partite. La natura schema-less di MongoDB inoltre mi ha permesso di ottimizzare le operazioni di lettura/scrittura per dati che presentano variazioni frequenti e che beneficiano di una modellazione meno rigida, inoltre ho deciso di suddividere in routes i gruppi di dati simili e utilizzare i modelli che si riferiscono ai dati nel database. Inoltre ho definito due controllers per le presenze e le partite nelle quali vengono definite due funzioni per ottenere tutte le presenze nel database e tutte le partite presenti inserendo come parametro l'id della partita per quest'ultima funzione. Ho creato in aggiunta anche i modelli delle tabelle del database, utilizzati dalle routes.</t>
-  </si>
-  <si>
     <t>Ho definito lo Springboot server inserendo al suo interno 4 moduli, uno per tabella presente nel database PostgreSQL, contenente le classi generiche, le interfacce e i servizi per ognuna di esse ( ne parlerò in dettaglio nella sezione della jpa ) più un singolo controller valido per tutti i moduli piuttosto che crearne uno per ognuno di essi, snellendo di fatto il codice e aumentando la facilità nella correzione di eventuali errori. Lo springbootserver presenta inoltre la classe WebConfig che configura il CORS o Cross Origin Resource Sharing per il server stesso definendo le origini delle richieste permesse ( in questo caso localhost:3000 - l'indirizzo del client ) e i metodi permessi per le richieste fatte dai servizi del client, ovvero "POST", "GET", "PUT",  e "DELETE".</t>
   </si>
   <si>
@@ -264,7 +255,13 @@
     <t>Si, per ogni funzione, componente, richiesta, route ecc.. Ho inserito commenti e documentazione javadoc</t>
   </si>
   <si>
+    <t>Si, ho utilizzato inizialmente yaml ma poi sono passato all'utilizzo di json per i file della documentazione poiché molto più rapidi e di maggior qualità</t>
+  </si>
+  <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t>Per quanto riguarda MongoDB, ho utilizzato tale database per memorizzare dati dinamici e in rapida evoluzione, quali i dettagli delle partite, gli eventi di gioco, le partite dei club e le prestazioni dei giocatori nelle partite. La natura schema-less di MongoDB inoltre mi ha permesso di ottimizzare le operazioni di lettura/scrittura per dati che presentano variazioni frequenti e che beneficiano di una modellazione meno rigida, inoltre ho deciso di suddividere in routes i gruppi di dati simili e utilizzare i modelli che si riferiscono ai dati nel database. Inoltre ho definito due controllers per le presenze e le partite nelle quali vengono definite due funzioni per ottenere tutte le presenze nel database e tutte le partite presenti nel database. Per quest'ultima, tramite il metodo find(), ho deciso di prendere tutti i dati presenti nel db a partire dalla stagione "2012". Ho creato in aggiunta anche i modelli delle tabelle del database, utilizzati dalle routes.</t>
   </si>
 </sst>
 </file>
@@ -958,8 +955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A704EA58-8849-E44F-8AE0-CB0AA8314588}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.4"/>
@@ -1093,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.4">
@@ -1174,7 +1171,7 @@
       </c>
       <c r="D27" s="5"/>
       <c r="E27" s="42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.4">
@@ -1204,7 +1201,7 @@
       </c>
       <c r="C31" s="4"/>
       <c r="D31">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.4">
@@ -1213,10 +1210,7 @@
       </c>
       <c r="C32" s="4"/>
       <c r="D32">
-        <v>2</v>
-      </c>
-      <c r="E32" s="41" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="64" x14ac:dyDescent="0.4">
@@ -1272,7 +1266,7 @@
         <v>18</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
@@ -1305,16 +1299,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="77.5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B45" s="32" t="s">
         <v>14</v>
       </c>
       <c r="C45" s="20"/>
       <c r="D45">
         <v>3</v>
-      </c>
-      <c r="E45" s="41" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="256" x14ac:dyDescent="0.4">
@@ -1325,7 +1316,7 @@
         <v>21</v>
       </c>
       <c r="E46" s="41" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
@@ -1402,7 +1393,7 @@
         <v>18</v>
       </c>
       <c r="E55" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.4">
@@ -1452,7 +1443,7 @@
         <v>21</v>
       </c>
       <c r="E60" s="41" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.4">
@@ -1468,7 +1459,7 @@
         <v>3</v>
       </c>
       <c r="E65" s="41" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="48" x14ac:dyDescent="0.4">
@@ -1477,6 +1468,9 @@
       </c>
       <c r="D66">
         <v>3</v>
+      </c>
+      <c r="E66" s="41" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.4">
@@ -1511,7 +1505,7 @@
       </c>
       <c r="C71" s="39"/>
       <c r="E71" s="41" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.4">

</xml_diff>